<commit_message>
updated list with status, incomplete
</commit_message>
<xml_diff>
--- a/Documents/Target_Satellite_List.xlsx
+++ b/Documents/Target_Satellite_List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tibbs2010\Desktop\SD\trunk\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lifesatrip\Documents\TortoiseSVN\SD\trunk\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,6 +23,357 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>lifesatrip</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Brandon:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Status</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Telemetry only
+10.35 days on followed by 10.35 days off.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Brandon:
+Status</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Just downlink</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Brandon:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Status</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Active only as digipeater</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Brandon:
+Status</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+TIsat-1 is still performing well after 19 months life in space. Due to some thermal issue (the reason of this is not clear yet) TIsat-1 is downloading data on the southern hemisphere. On the northern hemisphere we have beacon signals.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Brandon:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Status
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>CW telemetry only</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Brandon:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Status</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+CW beacon active G only about Japan</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Brandon:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Status</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+CW is the default mode of PRISM, the packet downlink will be active only in the command station in Japan.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Brandon:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Status</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+active in sunlight (but weak)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Brandon:
+Status</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+TIsat-1 is still performing well after 19 months life in space. Due to some thermal issue (the reason of this is not clear yet) TIsat-1 is downloading data on the southern hemisphere. On the northern hemisphere we have beacon signals.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
@@ -65,9 +416,6 @@
     <t>AO-71</t>
   </si>
   <si>
-    <t>EIP-71</t>
-  </si>
-  <si>
     <t>HORYU-2</t>
   </si>
   <si>
@@ -84,13 +432,16 @@
   </si>
   <si>
     <t>TISat-1</t>
+  </si>
+  <si>
+    <t>EIP-U2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,13 +449,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -128,9 +517,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,11 +801,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,25 +830,25 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-    </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
@@ -470,7 +861,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -480,7 +871,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -501,25 +892,27 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-    </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>19</v>
+      <c r="A15" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>